<commit_message>
Update to excel output
Fixing bug where excel was outputing journal and taccounts together
</commit_message>
<xml_diff>
--- a/LeapLog/bin/Debug/netcoreapp3.1/tigerllc.xlsx
+++ b/LeapLog/bin/Debug/netcoreapp3.1/tigerllc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/139cebc20cf1c155/01LoneStar/2020Spring/INEW2332Project/NewGit/leaplog/LeapLog/bin/Debug/netcoreapp3.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B359B86-5EAF-49C8-8D3C-9771CDAF18D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11961354-8E3E-4D0A-BB4C-F7700FB516A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2730" windowWidth="21600" windowHeight="12735" xr2:uid="{7C6F28B8-CF18-416F-8740-F6C4646C27DB}"/>
+    <workbookView xWindow="4245" yWindow="2580" windowWidth="21600" windowHeight="12735" xr2:uid="{1B5E6E1D-AF48-4658-91BF-61EFFB925937}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Owner Equity" sheetId="5" r:id="rId1"/>
@@ -574,8 +574,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1C33C5-5851-4104-85EC-15C35EF138F4}">
-  <dimension ref="A1:E44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68ABA057-92FD-45FD-A194-73E84D09E921}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -607,647 +607,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1">
-        <v>0</v>
-      </c>
-      <c r="C37" s="1">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1">
-        <v>0</v>
-      </c>
-      <c r="C38" s="1">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1">
-        <v>0</v>
-      </c>
-      <c r="E38" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1">
-        <v>0</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0</v>
-      </c>
-      <c r="D39" s="1">
-        <v>0</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1">
-        <v>0</v>
-      </c>
-      <c r="C41" s="1">
         <v>-1</v>
       </c>
-      <c r="D41" s="1">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1">
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3">
         <v>52</v>
       </c>
-      <c r="D42" s="1">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
         <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1">
-        <v>0</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1">
-        <v>0</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3">
-        <v>0</v>
-      </c>
-      <c r="C44" s="3">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1256,8 +633,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CBE465-EA62-4EC6-8110-81CC2DB1031D}">
-  <dimension ref="A1:D44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5185119-1962-4DBF-BC67-F16C9FB21B75}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1286,517 +663,23 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1">
-        <v>12</v>
-      </c>
-      <c r="C37" s="1">
-        <v>13</v>
-      </c>
-      <c r="D37" s="1">
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3">
         <v>52</v>
       </c>
-      <c r="C38" s="1">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
         <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1">
-        <v>0</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0</v>
-      </c>
-      <c r="D39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1">
-        <v>0</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1">
-        <v>0</v>
-      </c>
-      <c r="C42" s="1">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1">
-        <v>0</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3">
-        <v>0</v>
-      </c>
-      <c r="C44" s="3">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1805,8 +688,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84B79FB-56A3-4519-AA90-1B995943E254}">
-  <dimension ref="A1:G44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CFFE12-C3AE-4387-BF82-A59C0D038977}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1844,576 +727,40 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1"/>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="3">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1">
-        <v>0</v>
-      </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1">
-        <v>0</v>
-      </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="1">
-        <v>12</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="1">
-        <v>12</v>
-      </c>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
+      <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="1">
-        <v>12</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1" t="s">
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="1">
-        <v>12</v>
-      </c>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1">
-        <v>0</v>
-      </c>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1">
-        <v>0</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1">
-        <v>0</v>
-      </c>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1">
-        <v>0</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1">
-        <v>0</v>
-      </c>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1">
-        <v>0</v>
-      </c>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3">
-        <v>0</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3">
-        <v>0</v>
-      </c>
-      <c r="G44" s="3"/>
+      <c r="F4">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2421,8 +768,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D065B4-4B66-4F69-ACF6-9D16A76AA84B}">
-  <dimension ref="A1:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C024B04-2ACD-481F-B0D2-58A7D0662FBA}">
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3348,23 +1695,103 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3">
-        <v>0</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0</v>
-      </c>
-      <c r="F44" s="3">
-        <v>0</v>
-      </c>
-      <c r="G44" s="3">
-        <v>0</v>
-      </c>
-      <c r="H44" s="3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
         <v>0</v>
       </c>
     </row>
@@ -3374,8 +1801,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC07A877-A5D7-4B97-B254-177F9C7ACD07}">
-  <dimension ref="A1:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A640B038-200C-4337-88D3-AD164992554C}">
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4290,17 +2717,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3">
-        <v>0</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed "add journal" button name to "add database" and other user interfaces with that name as well.
</commit_message>
<xml_diff>
--- a/LeapLog/bin/Debug/netcoreapp3.1/tigerllc.xlsx
+++ b/LeapLog/bin/Debug/netcoreapp3.1/tigerllc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/139cebc20cf1c155/01LoneStar/2020Spring/INEW2332Project/NewGit/leaplog/LeapLog/bin/Debug/netcoreapp3.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D518535-5D02-48BE-8BF2-6B39ED06CB42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{97F0A383-825B-48A6-88F3-F10BA7E321ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C220458B-E0DB-4153-BC40-09C0F6A64DC4}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="2580" windowWidth="21600" windowHeight="12735" xr2:uid="{E2718743-751E-43CE-A178-FE8210CC7638}"/>
+    <workbookView xWindow="4245" yWindow="2580" windowWidth="21600" windowHeight="12735" activeTab="4" xr2:uid="{A5A86D8C-32C8-44A7-8787-94B6D784CDD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Owner Equity" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>Liability</t>
+  </si>
+  <si>
+    <t>NewEntry</t>
+  </si>
+  <si>
+    <t>OldEntry</t>
   </si>
 </sst>
 </file>
@@ -207,8 +213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -530,10 +538,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52DB3E8-E654-433B-AE3D-33F04CEECA69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6598E2D8-FAD2-413C-A269-2484DCA34002}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -545,19 +553,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -567,7 +575,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29F3AF5-E26A-4E12-AC73-D31E9CD03712}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E594F5E5-534D-4C1A-A0B5-07457BBD89B6}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -581,16 +589,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -600,8 +608,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1751B45-CD04-499C-8B21-CDDD994C4158}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BBA96E-63F1-41D7-BF9B-D751D9CB2DFA}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -616,27 +624,48 @@
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45</v>
+      </c>
+      <c r="G2" s="3">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -645,16 +674,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B0EF2D-3E69-45C4-852C-B9A99BC41249}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91965BE-2A87-4857-A8BF-0D3295F08DC2}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -663,29 +692,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>45</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -694,16 +746,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A928187-CC52-4986-9BF8-DC80A0221A71}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368653B6-58EB-4689-82FE-8DE7ADDCBD91}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -712,32 +764,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2">
         <v>43958</v>
@@ -759,6 +811,30 @@
       </c>
       <c r="H2" s="1">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4">
+        <v>43958</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="3">
+        <v>45</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>